<commit_message>
added operation dummy to port data
</commit_message>
<xml_diff>
--- a/Chinese_investments_14 Dec 23.xlsx
+++ b/Chinese_investments_14 Dec 23.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="11208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6888"/>
   </bookViews>
   <sheets>
     <sheet name="treatment_active" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="319">
   <si>
     <t>Portname</t>
   </si>
@@ -1062,6 +1062,12 @@
   </si>
   <si>
     <t>TRAMB</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>operation</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1343,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1602,7 +1608,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1919,745 +1926,770 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="74.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="106" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="106" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="106" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="106" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="106" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="106" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" style="106" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="106" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="74.6640625" style="106" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="106"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="106" t="s">
         <v>315</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="106" t="s">
         <v>244</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="106" t="s">
         <v>245</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="106" t="s">
         <v>314</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="106" t="s">
         <v>248</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="106" t="s">
         <v>249</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="106" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+      <c r="J1" s="106" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="106" t="s">
         <v>276</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="106">
         <v>2002</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="106">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="106" t="s">
         <v>258</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="106">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="106" t="s">
         <v>259</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="106" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="106" t="s">
         <v>310</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="106">
         <v>2013</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="106">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="106">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="106" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="J3" s="106" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="106" t="s">
         <v>293</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="106">
         <v>1983</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="106">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="106" t="s">
         <v>270</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="106">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="106" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="106">
         <v>2023</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="106">
         <v>2</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="107" t="s">
         <v>260</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="106">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="106" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+      <c r="J5" s="106" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="106" t="s">
         <v>291</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="106">
         <v>2012</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="106">
         <v>3</v>
       </c>
-      <c r="F6" s="106" t="s">
+      <c r="F6" s="107" t="s">
         <v>268</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="106">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="106" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="106" t="s">
         <v>307</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="106">
         <v>2017</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="106">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="106">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="106" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="106" t="s">
         <v>292</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="106">
         <v>2017</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="106">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="106">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="106" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="106" t="s">
         <v>299</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="106">
         <v>2013</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="106">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="106">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="106" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" s="106" t="s">
         <v>302</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="106" t="s">
         <v>266</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="106">
         <v>2013</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="106">
         <v>2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="106">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="106" t="s">
         <v>256</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="106" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10">
+      <c r="A11" s="106" t="s">
         <v>294</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="106">
         <v>2013</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="106">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="106">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="106" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10">
+      <c r="A12" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="106" t="s">
         <v>267</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="106">
         <v>2013</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="106">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="106">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="106" t="s">
         <v>256</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="106" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="106">
         <v>1991</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="106">
         <v>3</v>
       </c>
-      <c r="F13" s="106" t="s">
+      <c r="F13" s="107" t="s">
         <v>275</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="106">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="106" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10">
+      <c r="A14" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="106" t="s">
         <v>281</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="106">
         <v>1998</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="106">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="106" t="s">
         <v>282</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="106">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="106" t="s">
         <v>259</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="106" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15" s="106" t="s">
         <v>312</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="106" t="s">
         <v>202</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="106">
         <v>1998</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="106">
         <v>2</v>
       </c>
-      <c r="F15" s="106" t="s">
+      <c r="F15" s="107" t="s">
         <v>273</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="106">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="106" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" s="106" t="s">
         <v>303</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="106">
         <v>2009</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="106">
         <v>4</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="106" t="s">
         <v>251</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="106">
         <v>1</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="106" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
+      <c r="J16" s="106" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="106" t="s">
         <v>306</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="106">
         <v>2018</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="106">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="106" t="s">
         <v>265</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="106">
         <v>1</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="106" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
+    <row r="18" spans="1:10">
+      <c r="A18" s="106" t="s">
         <v>297</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="106" t="s">
         <v>254</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="106">
         <v>2017</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="106">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="106">
         <v>1</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="106" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
+      <c r="J18" s="106" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="106" t="s">
         <v>300</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="106">
         <v>2013</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="106">
         <v>2</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="106">
         <v>1</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="106" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10">
+      <c r="A20" s="106" t="s">
         <v>304</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="106">
         <v>2002</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="106">
         <v>1</v>
       </c>
-      <c r="F20" s="106" t="s">
+      <c r="F20" s="107" t="s">
         <v>258</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="106">
         <v>3</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="106" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
+      <c r="J20" s="106" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="106" t="s">
         <v>301</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="106">
         <v>2002</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="106">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="106" t="s">
         <v>258</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="106">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="106" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
+      <c r="J21" s="106" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="106" t="s">
         <v>290</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="106">
         <v>2004</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="106">
         <v>4</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="106" t="s">
         <v>257</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="106">
         <v>3</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="106" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
+    <row r="23" spans="1:10">
+      <c r="A23" s="106" t="s">
         <v>308</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="106" t="s">
         <v>278</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="106">
         <v>2010</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="106">
         <v>2</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="106" t="s">
         <v>279</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="106">
         <v>1</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="106" t="s">
         <v>259</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="106" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="106" t="s">
         <v>289</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="106" t="s">
         <v>114</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="106">
         <v>2018</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="106">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="106" t="s">
         <v>269</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="106">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="106" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" s="106" t="s">
         <v>296</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="106" t="s">
         <v>119</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="106">
         <v>2006</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="106">
         <v>2</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="106" t="s">
         <v>272</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="106">
         <v>1</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="106" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="106" t="s">
         <v>305</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="106" t="s">
         <v>118</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="106">
         <v>2009</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="106">
         <v>1</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="106">
         <v>1</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="106" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
+      <c r="J26" s="106" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="106" t="s">
         <v>316</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="106" t="s">
         <v>261</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="106">
         <v>2015</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="106">
         <v>4</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="106" t="s">
         <v>262</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="106">
         <v>2</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="106" t="s">
         <v>263</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="106" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2756,7 +2788,7 @@
   <dimension ref="A1:O643"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -7302,7 +7334,7 @@
   <dimension ref="A1:Q628"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -11575,8 +11607,8 @@
   </sheetPr>
   <dimension ref="A1:N616"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A7" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
added extensions to estimation file
</commit_message>
<xml_diff>
--- a/Chinese_investments_14 Dec 23.xlsx
+++ b/Chinese_investments_14 Dec 23.xlsx
@@ -1064,10 +1064,10 @@
     <t>TRAMB</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>operation</t>
+  </si>
+  <si>
+    <t>investment_type</t>
   </si>
 </sst>
 </file>
@@ -1929,7 +1929,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1975,7 +1975,7 @@
         <v>288</v>
       </c>
       <c r="J1" s="106" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2033,7 +2033,7 @@
         <v>256</v>
       </c>
       <c r="J3" s="106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2088,7 +2088,7 @@
         <v>252</v>
       </c>
       <c r="J5" s="106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2386,7 +2386,7 @@
         <v>252</v>
       </c>
       <c r="J16" s="106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2441,7 +2441,7 @@
         <v>252</v>
       </c>
       <c r="J18" s="106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2496,7 +2496,7 @@
         <v>259</v>
       </c>
       <c r="J20" s="106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2525,7 +2525,7 @@
         <v>259</v>
       </c>
       <c r="J21" s="106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2661,7 +2661,7 @@
         <v>259</v>
       </c>
       <c r="J26" s="106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2788,7 +2788,7 @@
   <dimension ref="A1:O643"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
update Savona instead of Genova treatment
</commit_message>
<xml_diff>
--- a/Chinese_investments_14 Dec 23.xlsx
+++ b/Chinese_investments_14 Dec 23.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHK\Documents\Projekte\China_European Ports\European-Ports-Ownership\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalkschmied\Desktop\Forschung\European ports development with Paul Stricker\Analysis\Ports analysis - github\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E051EAF7-A5B5-489C-8FF3-EB7FE6E7B6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6888"/>
+    <workbookView xWindow="-21435" yWindow="5850" windowWidth="19425" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="treatment_active" sheetId="4" r:id="rId1"/>
@@ -22,17 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -875,9 +865,6 @@
     <t>Q2</t>
   </si>
   <si>
-    <t>Genova</t>
-  </si>
-  <si>
     <t>11 June 2013</t>
   </si>
   <si>
@@ -1004,9 +991,6 @@
     <t>PLGDY</t>
   </si>
   <si>
-    <t>ITGOA</t>
-  </si>
-  <si>
     <t>DEHAM</t>
   </si>
   <si>
@@ -1068,17 +1052,23 @@
   </si>
   <si>
     <t>investment_type</t>
+  </si>
+  <si>
+    <t>Savona</t>
+  </si>
+  <si>
+    <t>ITSVN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="167" formatCode="[$£-809]#,##0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="[$£-809]#,##0"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -1340,7 +1330,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="108">
@@ -1408,7 +1398,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1444,7 +1434,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1495,7 +1485,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1507,14 +1497,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1574,7 +1564,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1612,9 +1602,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1925,30 +1915,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" style="106" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" style="106" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="106" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="106" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6328125" style="106" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="106" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="106" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.36328125" style="106" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="106" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="106" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" style="106" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="106" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="74.6640625" style="106" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="106"/>
+    <col min="9" max="9" width="74.6328125" style="106" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="106"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="106" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B1" s="106" t="s">
         <v>244</v>
@@ -1960,7 +1950,7 @@
         <v>246</v>
       </c>
       <c r="E1" s="106" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F1" s="106" t="s">
         <v>247</v>
@@ -1972,18 +1962,18 @@
         <v>249</v>
       </c>
       <c r="I1" s="106" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J1" s="106" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="106" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B2" s="106" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="106" t="s">
         <v>38</v>
@@ -1995,21 +1985,21 @@
         <v>1</v>
       </c>
       <c r="F2" s="106" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G2" s="106">
         <v>1</v>
       </c>
       <c r="H2" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I2" s="106" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="106" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B3" s="106" t="s">
         <v>37</v>
@@ -2024,21 +2014,21 @@
         <v>2</v>
       </c>
       <c r="F3" s="106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G3" s="106">
         <v>2</v>
       </c>
       <c r="H3" s="106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J3" s="106" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="106" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B4" s="106" t="s">
         <v>116</v>
@@ -2053,18 +2043,18 @@
         <v>1</v>
       </c>
       <c r="F4" s="106" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G4" s="106">
         <v>1</v>
       </c>
       <c r="H4" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="106" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B5" s="106" t="s">
         <v>44</v>
@@ -2079,7 +2069,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G5" s="106">
         <v>1</v>
@@ -2088,12 +2078,12 @@
         <v>252</v>
       </c>
       <c r="J5" s="106" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="106" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B6" s="106" t="s">
         <v>112</v>
@@ -2108,18 +2098,18 @@
         <v>3</v>
       </c>
       <c r="F6" s="107" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G6" s="106">
         <v>1</v>
       </c>
       <c r="H6" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="106" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B7" s="106" t="s">
         <v>26</v>
@@ -2145,7 +2135,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="106" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B8" s="106" t="s">
         <v>31</v>
@@ -2171,7 +2161,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="106" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B9" s="106" t="s">
         <v>75</v>
@@ -2186,21 +2176,21 @@
         <v>2</v>
       </c>
       <c r="F9" s="106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G9" s="106">
         <v>1</v>
       </c>
       <c r="H9" s="106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="106" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B10" s="106" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C10" s="106" t="s">
         <v>76</v>
@@ -2212,13 +2202,13 @@
         <v>2</v>
       </c>
       <c r="F10" s="106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G10" s="106">
         <v>1</v>
       </c>
       <c r="H10" s="106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I10" s="106" t="s">
         <v>224</v>
@@ -2226,7 +2216,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="106" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B11" s="106" t="s">
         <v>74</v>
@@ -2241,21 +2231,21 @@
         <v>2</v>
       </c>
       <c r="F11" s="106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G11" s="106">
         <v>1</v>
       </c>
       <c r="H11" s="106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="106" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B12" s="106" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>76</v>
@@ -2267,13 +2257,13 @@
         <v>2</v>
       </c>
       <c r="F12" s="106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G12" s="106">
         <v>1</v>
       </c>
       <c r="H12" s="106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I12" s="106" t="s">
         <v>225</v>
@@ -2281,10 +2271,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="106" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B13" s="106" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C13" s="106" t="s">
         <v>177</v>
@@ -2296,21 +2286,21 @@
         <v>3</v>
       </c>
       <c r="F13" s="107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G13" s="106">
         <v>1</v>
       </c>
       <c r="H13" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="106" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C14" s="106" t="s">
         <v>177</v>
@@ -2322,21 +2312,21 @@
         <v>1</v>
       </c>
       <c r="F14" s="106" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G14" s="106">
         <v>1</v>
       </c>
       <c r="H14" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I14" s="106" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="106" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B15" s="106" t="s">
         <v>202</v>
@@ -2351,18 +2341,18 @@
         <v>2</v>
       </c>
       <c r="F15" s="107" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G15" s="106">
         <v>1</v>
       </c>
       <c r="H15" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="106" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B16" s="106" t="s">
         <v>4</v>
@@ -2386,12 +2376,12 @@
         <v>252</v>
       </c>
       <c r="J16" s="106" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="106" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B17" s="106" t="s">
         <v>17</v>
@@ -2406,21 +2396,21 @@
         <v>1</v>
       </c>
       <c r="F17" s="106" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G17" s="106">
         <v>1</v>
       </c>
       <c r="H17" s="106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="106" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
       <c r="B18" s="106" t="s">
-        <v>254</v>
+        <v>317</v>
       </c>
       <c r="C18" s="106" t="s">
         <v>35</v>
@@ -2441,12 +2431,12 @@
         <v>252</v>
       </c>
       <c r="J18" s="106" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="106" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B19" s="106" t="s">
         <v>98</v>
@@ -2461,18 +2451,18 @@
         <v>2</v>
       </c>
       <c r="F19" s="106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G19" s="106">
         <v>1</v>
       </c>
       <c r="H19" s="106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="106" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B20" s="106" t="s">
         <v>40</v>
@@ -2487,21 +2477,21 @@
         <v>1</v>
       </c>
       <c r="F20" s="107" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G20" s="106">
         <v>3</v>
       </c>
       <c r="H20" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J20" s="106" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="106" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B21" s="106" t="s">
         <v>115</v>
@@ -2516,21 +2506,21 @@
         <v>1</v>
       </c>
       <c r="F21" s="106" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G21" s="106">
         <v>1</v>
       </c>
       <c r="H21" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J21" s="106" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="106" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B22" s="106" t="s">
         <v>39</v>
@@ -2545,7 +2535,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="106" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G22" s="106">
         <v>3</v>
@@ -2556,10 +2546,10 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="106" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B23" s="106" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>41</v>
@@ -2571,21 +2561,21 @@
         <v>2</v>
       </c>
       <c r="F23" s="106" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G23" s="106">
         <v>1</v>
       </c>
       <c r="H23" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I23" s="106" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="106" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B24" s="106" t="s">
         <v>114</v>
@@ -2600,18 +2590,18 @@
         <v>1</v>
       </c>
       <c r="F24" s="106" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G24" s="106">
         <v>1</v>
       </c>
       <c r="H24" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="106" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B25" s="106" t="s">
         <v>119</v>
@@ -2626,18 +2616,18 @@
         <v>2</v>
       </c>
       <c r="F25" s="106" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G25" s="106">
         <v>1</v>
       </c>
       <c r="H25" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="106" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B26" s="106" t="s">
         <v>117</v>
@@ -2652,24 +2642,24 @@
         <v>1</v>
       </c>
       <c r="F26" s="106" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G26" s="106">
         <v>1</v>
       </c>
       <c r="H26" s="106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J26" s="106" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="106" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B27" s="106" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C27" s="106" t="s">
         <v>48</v>
@@ -2681,20 +2671,20 @@
         <v>4</v>
       </c>
       <c r="F27" s="106" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G27" s="106">
         <v>2</v>
       </c>
       <c r="H27" s="106" t="s">
+        <v>262</v>
+      </c>
+      <c r="I27" s="106" t="s">
         <v>263</v>
       </c>
-      <c r="I27" s="106" t="s">
-        <v>264</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I28">
     <sortCondition ref="C2:C28"/>
     <sortCondition ref="D2:D28"/>
     <sortCondition ref="E2:E28"/>
@@ -2705,19 +2695,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2731,16 +2721,16 @@
         <v>245</v>
       </c>
       <c r="D1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E1" t="s">
         <v>284</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>285</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>286</v>
-      </c>
-      <c r="G1" t="s">
-        <v>287</v>
       </c>
       <c r="H1" t="s">
         <v>248</v>
@@ -2781,7 +2771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -2791,23 +2781,23 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="149.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.109375" style="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="149.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" thickTop="1" thickBot="1">
+    <row r="1" spans="1:15" ht="15.5" thickTop="1" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +2883,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="31" customFormat="1" ht="43.2">
+    <row r="3" spans="1:15" s="31" customFormat="1" ht="43.5">
       <c r="A3" s="35" t="s">
         <v>4</v>
       </c>
@@ -2968,7 +2958,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="31" customFormat="1" ht="28.8">
+    <row r="5" spans="1:15" s="31" customFormat="1" ht="29">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
@@ -3013,7 +3003,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="31" customFormat="1" ht="72">
+    <row r="6" spans="1:15" s="31" customFormat="1" ht="72.5">
       <c r="A6" s="26" t="s">
         <v>31</v>
       </c>
@@ -3053,7 +3043,7 @@
       </c>
       <c r="N6" s="26"/>
     </row>
-    <row r="7" spans="1:15" s="31" customFormat="1" ht="57.6">
+    <row r="7" spans="1:15" s="31" customFormat="1" ht="58">
       <c r="A7" s="26" t="s">
         <v>34</v>
       </c>
@@ -3325,7 +3315,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="31" customFormat="1" ht="43.2">
+    <row r="14" spans="1:15" s="31" customFormat="1" ht="43.5">
       <c r="A14" s="26" t="s">
         <v>44</v>
       </c>
@@ -7273,53 +7263,53 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K5" r:id="rId1"/>
-    <hyperlink ref="L5" r:id="rId2"/>
-    <hyperlink ref="M5" r:id="rId3"/>
-    <hyperlink ref="K14" r:id="rId4"/>
-    <hyperlink ref="K15" r:id="rId5"/>
-    <hyperlink ref="M15" r:id="rId6"/>
-    <hyperlink ref="L15" r:id="rId7"/>
-    <hyperlink ref="N15" r:id="rId8"/>
-    <hyperlink ref="K12" r:id="rId9"/>
-    <hyperlink ref="K6" r:id="rId10"/>
-    <hyperlink ref="L6" r:id="rId11"/>
-    <hyperlink ref="K2" r:id="rId12"/>
-    <hyperlink ref="L2" r:id="rId13"/>
-    <hyperlink ref="M2" r:id="rId14"/>
-    <hyperlink ref="K3" r:id="rId15"/>
-    <hyperlink ref="K4" r:id="rId16"/>
-    <hyperlink ref="L4" r:id="rId17"/>
-    <hyperlink ref="L14" r:id="rId18"/>
-    <hyperlink ref="M14" r:id="rId19"/>
-    <hyperlink ref="K13" r:id="rId20"/>
-    <hyperlink ref="L13" r:id="rId21"/>
-    <hyperlink ref="L12" r:id="rId22"/>
-    <hyperlink ref="K10" r:id="rId23"/>
-    <hyperlink ref="K9" r:id="rId24"/>
-    <hyperlink ref="K8" r:id="rId25"/>
-    <hyperlink ref="L8" r:id="rId26"/>
-    <hyperlink ref="N5" r:id="rId27"/>
-    <hyperlink ref="N2" r:id="rId28"/>
-    <hyperlink ref="M4" r:id="rId29"/>
-    <hyperlink ref="O5" r:id="rId30"/>
-    <hyperlink ref="M6" r:id="rId31"/>
-    <hyperlink ref="K11" r:id="rId32"/>
-    <hyperlink ref="L11" r:id="rId33"/>
-    <hyperlink ref="M11" r:id="rId34"/>
-    <hyperlink ref="M13" r:id="rId35"/>
-    <hyperlink ref="N13" r:id="rId36"/>
-    <hyperlink ref="N14" r:id="rId37"/>
-    <hyperlink ref="O15" r:id="rId38"/>
-    <hyperlink ref="N8" r:id="rId39"/>
-    <hyperlink ref="L9" r:id="rId40"/>
-    <hyperlink ref="M9" r:id="rId41"/>
-    <hyperlink ref="K7" r:id="rId42"/>
-    <hyperlink ref="L7" r:id="rId43"/>
-    <hyperlink ref="M8" r:id="rId44"/>
-    <hyperlink ref="N7" r:id="rId45"/>
-    <hyperlink ref="N9" r:id="rId46"/>
-    <hyperlink ref="L10" r:id="rId47"/>
+    <hyperlink ref="K5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="L5" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="M5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="K14" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="K15" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="M15" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="L15" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="N15" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="K12" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="K6" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="L6" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="K2" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="L2" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="M2" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="K3" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="K4" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="L4" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="L14" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="M14" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="K13" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="L13" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="L12" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="K10" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="K9" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="K8" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="L8" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="N5" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="N2" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="M4" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="O5" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="M6" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="K11" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="L11" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="M11" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="M13" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="N13" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="N14" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="O15" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="N8" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="L9" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="M9" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="K7" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="L7" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="M8" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="N7" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="N9" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="L10" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId48"/>
@@ -7327,7 +7317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
@@ -7337,23 +7327,23 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1"/>
-    <col min="10" max="10" width="149.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.109375" style="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" customWidth="1"/>
+    <col min="10" max="10" width="149.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" thickTop="1" thickBot="1">
+    <row r="1" spans="1:17" ht="15.5" thickTop="1" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7397,7 +7387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" ht="144">
+    <row r="2" spans="1:17" s="31" customFormat="1" ht="145">
       <c r="A2" s="26" t="s">
         <v>17</v>
       </c>
@@ -7448,7 +7438,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="100.8">
+    <row r="3" spans="1:17" ht="101.5">
       <c r="A3" s="26" t="s">
         <v>98</v>
       </c>
@@ -11572,36 +11562,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="L2" r:id="rId2"/>
-    <hyperlink ref="K11" r:id="rId3"/>
-    <hyperlink ref="L11" r:id="rId4"/>
-    <hyperlink ref="M11" r:id="rId5"/>
-    <hyperlink ref="K3" r:id="rId6"/>
-    <hyperlink ref="L3" r:id="rId7"/>
-    <hyperlink ref="K6" r:id="rId8"/>
-    <hyperlink ref="K7" r:id="rId9"/>
-    <hyperlink ref="K8" r:id="rId10"/>
-    <hyperlink ref="L6" r:id="rId11"/>
-    <hyperlink ref="L7" r:id="rId12"/>
-    <hyperlink ref="L8" r:id="rId13"/>
-    <hyperlink ref="K4" r:id="rId14"/>
-    <hyperlink ref="K5" r:id="rId15"/>
-    <hyperlink ref="M5" r:id="rId16"/>
-    <hyperlink ref="K10" r:id="rId17" location="cite_note-:5-16"/>
-    <hyperlink ref="M3" r:id="rId18" location="cite_note-:5-16"/>
-    <hyperlink ref="M2" r:id="rId19"/>
-    <hyperlink ref="N2" r:id="rId20"/>
-    <hyperlink ref="O2" r:id="rId21"/>
-    <hyperlink ref="P2" r:id="rId22"/>
-    <hyperlink ref="Q2" r:id="rId23"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="K11" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="L11" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="M11" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="K3" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="L3" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="K6" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="K7" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="K8" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="L6" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="L7" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="L8" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="K4" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="K5" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="M5" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="K10" r:id="rId17" location="cite_note-:5-16" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="M3" r:id="rId18" location="cite_note-:5-16" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="M2" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="N2" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="O2" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="P2" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="Q2" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -11611,23 +11601,23 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1"/>
-    <col min="10" max="10" width="78.109375" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.109375" style="1"/>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="16.90625" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.08984375" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" customWidth="1"/>
+    <col min="10" max="10" width="78.08984375" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="31" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="1" spans="1:14" s="31" customFormat="1" ht="15.5" thickTop="1" thickBot="1">
       <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
@@ -11671,7 +11661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="31" customFormat="1" ht="43.2">
+    <row r="2" spans="1:14" s="31" customFormat="1" ht="43.5">
       <c r="A2" s="35" t="s">
         <v>112</v>
       </c>
@@ -11775,7 +11765,7 @@
       <c r="M4" s="60"/>
       <c r="N4" s="26"/>
     </row>
-    <row r="5" spans="1:14" s="31" customFormat="1" ht="43.2">
+    <row r="5" spans="1:14" s="31" customFormat="1" ht="58">
       <c r="A5" s="26" t="s">
         <v>39</v>
       </c>
@@ -11805,7 +11795,7 @@
       <c r="M5" s="26"/>
       <c r="N5" s="26"/>
     </row>
-    <row r="6" spans="1:14" s="31" customFormat="1" ht="72">
+    <row r="6" spans="1:14" s="31" customFormat="1" ht="72.5">
       <c r="A6" s="26" t="s">
         <v>114</v>
       </c>
@@ -11871,7 +11861,7 @@
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
     </row>
-    <row r="8" spans="1:14" s="31" customFormat="1" ht="129.6">
+    <row r="8" spans="1:14" s="31" customFormat="1" ht="130.5">
       <c r="A8" s="26" t="s">
         <v>116</v>
       </c>
@@ -12074,7 +12064,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:14" s="81" customFormat="1" ht="28.8">
+    <row r="15" spans="1:14" s="81" customFormat="1" ht="29">
       <c r="A15" s="73" t="s">
         <v>206</v>
       </c>
@@ -12108,7 +12098,7 @@
       <c r="M15" s="80"/>
       <c r="N15" s="80"/>
     </row>
-    <row r="16" spans="1:14" s="81" customFormat="1" ht="115.2">
+    <row r="16" spans="1:14" s="81" customFormat="1" ht="116">
       <c r="A16" s="80" t="s">
         <v>208</v>
       </c>
@@ -15827,32 +15817,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="L2" r:id="rId2" location="cite_note-sub-14"/>
-    <hyperlink ref="K3" r:id="rId3" location="cite_note-sub-14"/>
-    <hyperlink ref="K10" r:id="rId4"/>
-    <hyperlink ref="K9" r:id="rId5" location="/Home"/>
-    <hyperlink ref="K8" r:id="rId6"/>
-    <hyperlink ref="K7" r:id="rId7"/>
-    <hyperlink ref="K16" r:id="rId8"/>
-    <hyperlink ref="M2" r:id="rId9"/>
-    <hyperlink ref="L3" r:id="rId10"/>
-    <hyperlink ref="K4" r:id="rId11"/>
-    <hyperlink ref="K6" r:id="rId12"/>
-    <hyperlink ref="L7" r:id="rId13"/>
-    <hyperlink ref="L9" r:id="rId14"/>
-    <hyperlink ref="M9" r:id="rId15"/>
-    <hyperlink ref="L10" r:id="rId16"/>
-    <hyperlink ref="K11" r:id="rId17"/>
-    <hyperlink ref="L11" r:id="rId18"/>
-    <hyperlink ref="K12" r:id="rId19"/>
-    <hyperlink ref="L12" r:id="rId20"/>
-    <hyperlink ref="M10" r:id="rId21"/>
-    <hyperlink ref="L15" r:id="rId22"/>
-    <hyperlink ref="K15" r:id="rId23" location="cite_note-sub-14"/>
-    <hyperlink ref="L6" r:id="rId24" display="https://www.hutchisonportsduisburg.de/en/hutchison-ports-duisburg-celebrates-its-40th-anniversary"/>
-    <hyperlink ref="K17" r:id="rId25"/>
-    <hyperlink ref="L17" r:id="rId26"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="L2" r:id="rId2" location="cite_note-sub-14" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="K3" r:id="rId3" location="cite_note-sub-14" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="K10" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="K9" r:id="rId5" location="/Home" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="K8" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="K7" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="K16" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="M2" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="L3" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="K4" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="K6" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="L7" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="L9" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="M9" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="L10" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="K11" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="L11" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="K12" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="L12" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="M10" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="L15" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="K15" r:id="rId23" location="cite_note-sub-14" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="L6" r:id="rId24" display="https://www.hutchisonportsduisburg.de/en/hutchison-ports-duisburg-celebrates-its-40th-anniversary" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="K17" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="L17" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Savona instead of Genova treatment
</commit_message>
<xml_diff>
--- a/Chinese_investments_14 Dec 23.xlsx
+++ b/Chinese_investments_14 Dec 23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalkschmied\Desktop\Forschung\European ports development with Paul Stricker\Analysis\Ports analysis - github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E051EAF7-A5B5-489C-8FF3-EB7FE6E7B6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D6421C-6436-4B07-9419-5542D294D5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21435" yWindow="5850" windowWidth="19425" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21435" yWindow="5775" windowWidth="19425" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="treatment_active" sheetId="4" r:id="rId1"/>

</xml_diff>